<commit_message>
pop-up that allows to save xlsx is working
</commit_message>
<xml_diff>
--- a/mvc/controllers/consult/chart_report.xlsx
+++ b/mvc/controllers/consult/chart_report.xlsx
@@ -140,7 +140,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:t>Cantidad de Alumnos</a:t>
+              <a:t>Students' Entrances</a:t>
             </a:r>
           </a:p>
         </rich>
@@ -556,7 +556,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -578,15 +578,15 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>44986</v>
+        <v>45013</v>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>44987</v>
+        <v>44986</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
@@ -594,7 +594,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>44988</v>
+        <v>44987</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
@@ -602,7 +602,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>44989</v>
+        <v>44988</v>
       </c>
       <c r="B5" t="n">
         <v>1</v>
@@ -610,9 +610,17 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
+        <v>44989</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
         <v>44990</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B7" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>